<commit_message>
initial display is finished - commencing js functionality
</commit_message>
<xml_diff>
--- a/excelparser_v1/files/exliste.xlsx
+++ b/excelparser_v1/files/exliste.xlsx
@@ -2803,22 +2803,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A157" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E165" sqref="E165"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="62.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="65" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" customWidth="1"/>
+    <col min="7" max="7" width="31.33203125" customWidth="1"/>
     <col min="8" max="8" width="126" customWidth="1"/>
     <col min="10" max="10" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2850,7 +2850,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>721</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>711</v>
       </c>
@@ -2899,7 +2899,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>711</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -3169,7 +3169,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -3265,7 +3265,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -3393,7 +3393,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -3521,7 +3521,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -3634,7 +3634,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -3666,7 +3666,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -3698,7 +3698,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -3730,7 +3730,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -3762,7 +3762,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -3794,7 +3794,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -3826,7 +3826,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -3858,7 +3858,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -3890,7 +3890,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -3954,7 +3954,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -4050,7 +4050,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -4082,7 +4082,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -4178,7 +4178,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>10</v>
       </c>
@@ -4210,7 +4210,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -4242,7 +4242,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>1</v>
       </c>
@@ -4259,7 +4259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>11</v>
       </c>
@@ -4291,7 +4291,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>11</v>
       </c>
@@ -4323,7 +4323,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>11</v>
       </c>
@@ -4355,7 +4355,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -4387,7 +4387,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -4419,7 +4419,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -4451,7 +4451,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -4483,7 +4483,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -4515,7 +4515,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>13</v>
       </c>
@@ -4547,7 +4547,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>13</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>13</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>13</v>
       </c>
@@ -4643,7 +4643,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>14</v>
       </c>
@@ -4675,7 +4675,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -4707,7 +4707,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -4739,7 +4739,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>15</v>
       </c>
@@ -4759,7 +4759,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>16</v>
       </c>
@@ -4776,7 +4776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>17</v>
       </c>
@@ -4808,7 +4808,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>17</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>17</v>
       </c>
@@ -4872,7 +4872,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>18</v>
       </c>
@@ -4904,7 +4904,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>18</v>
       </c>
@@ -4936,7 +4936,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>18</v>
       </c>
@@ -4968,7 +4968,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>18</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>19</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>19</v>
       </c>
@@ -5064,7 +5064,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>19</v>
       </c>
@@ -5096,7 +5096,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>19</v>
       </c>
@@ -5128,7 +5128,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>20</v>
       </c>
@@ -5160,7 +5160,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>20</v>
       </c>
@@ -5192,7 +5192,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>20</v>
       </c>
@@ -5224,7 +5224,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>20</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>21</v>
       </c>
@@ -5288,7 +5288,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>21</v>
       </c>
@@ -5320,7 +5320,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>21</v>
       </c>
@@ -5352,7 +5352,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>1</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>22</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>22</v>
       </c>
@@ -5433,7 +5433,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>22</v>
       </c>
@@ -5465,7 +5465,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>22</v>
       </c>
@@ -5497,7 +5497,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>23</v>
       </c>
@@ -5529,7 +5529,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>23</v>
       </c>
@@ -5561,7 +5561,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>23</v>
       </c>
@@ -5593,7 +5593,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>23</v>
       </c>
@@ -5625,7 +5625,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>24</v>
       </c>
@@ -5657,7 +5657,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>24</v>
       </c>
@@ -5689,7 +5689,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>24</v>
       </c>
@@ -5721,7 +5721,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>25</v>
       </c>
@@ -5753,7 +5753,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>25</v>
       </c>
@@ -5785,7 +5785,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>25</v>
       </c>
@@ -5817,7 +5817,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>25</v>
       </c>
@@ -5849,7 +5849,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>1</v>
       </c>
@@ -5866,7 +5866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>712</v>
       </c>
@@ -5895,7 +5895,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>712</v>
       </c>
@@ -5924,7 +5924,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>1</v>
       </c>
@@ -5941,7 +5941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>26</v>
       </c>
@@ -5973,7 +5973,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>26</v>
       </c>
@@ -6005,7 +6005,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>26</v>
       </c>
@@ -6037,7 +6037,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>26</v>
       </c>
@@ -6069,7 +6069,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>27</v>
       </c>
@@ -6101,7 +6101,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>27</v>
       </c>
@@ -6133,7 +6133,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>27</v>
       </c>
@@ -6165,7 +6165,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>27</v>
       </c>
@@ -6197,7 +6197,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>28</v>
       </c>
@@ -6229,7 +6229,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>28</v>
       </c>
@@ -6261,7 +6261,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>28</v>
       </c>
@@ -6293,7 +6293,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>28</v>
       </c>
@@ -6325,7 +6325,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>29</v>
       </c>
@@ -6357,7 +6357,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>29</v>
       </c>
@@ -6389,7 +6389,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>29</v>
       </c>
@@ -6421,7 +6421,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>30</v>
       </c>
@@ -6453,7 +6453,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>30</v>
       </c>
@@ -6485,7 +6485,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>30</v>
       </c>
@@ -6517,7 +6517,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>30</v>
       </c>
@@ -6549,7 +6549,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>1</v>
       </c>
@@ -6566,7 +6566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>31</v>
       </c>
@@ -6598,7 +6598,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>31</v>
       </c>
@@ -6630,7 +6630,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>31</v>
       </c>
@@ -6662,7 +6662,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>31</v>
       </c>
@@ -6694,7 +6694,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>32</v>
       </c>
@@ -6726,7 +6726,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>32</v>
       </c>
@@ -6758,7 +6758,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>32</v>
       </c>
@@ -6790,7 +6790,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>32</v>
       </c>
@@ -6822,7 +6822,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>33</v>
       </c>
@@ -6854,7 +6854,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>33</v>
       </c>
@@ -6886,7 +6886,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>33</v>
       </c>
@@ -6918,7 +6918,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>33</v>
       </c>
@@ -6950,7 +6950,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>34</v>
       </c>
@@ -6982,7 +6982,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>34</v>
       </c>
@@ -7014,7 +7014,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>34</v>
       </c>
@@ -7046,7 +7046,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>34</v>
       </c>
@@ -7078,7 +7078,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>35</v>
       </c>
@@ -7095,7 +7095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>36</v>
       </c>
@@ -7127,7 +7127,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>36</v>
       </c>
@@ -7159,7 +7159,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>36</v>
       </c>
@@ -7191,7 +7191,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>36</v>
       </c>
@@ -7223,7 +7223,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>36</v>
       </c>
@@ -7255,7 +7255,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>37</v>
       </c>
@@ -7287,7 +7287,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>37</v>
       </c>
@@ -7319,7 +7319,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>37</v>
       </c>
@@ -7351,7 +7351,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>38</v>
       </c>
@@ -7383,7 +7383,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>38</v>
       </c>
@@ -7415,7 +7415,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>38</v>
       </c>
@@ -7447,7 +7447,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>38</v>
       </c>
@@ -7479,7 +7479,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>39</v>
       </c>
@@ -7511,7 +7511,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>39</v>
       </c>
@@ -7543,7 +7543,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>39</v>
       </c>
@@ -7575,7 +7575,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>39</v>
       </c>
@@ -7607,7 +7607,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>1</v>
       </c>
@@ -7624,7 +7624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>40</v>
       </c>
@@ -7656,7 +7656,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>40</v>
       </c>
@@ -7688,7 +7688,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>40</v>
       </c>
@@ -7720,7 +7720,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>40</v>
       </c>
@@ -7752,7 +7752,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>41</v>
       </c>
@@ -7784,7 +7784,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>41</v>
       </c>
@@ -7816,7 +7816,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>41</v>
       </c>
@@ -7848,7 +7848,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>41</v>
       </c>
@@ -7880,7 +7880,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>42</v>
       </c>
@@ -7912,7 +7912,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>42</v>
       </c>
@@ -7944,7 +7944,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>42</v>
       </c>
@@ -7976,7 +7976,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>42</v>
       </c>
@@ -8008,7 +8008,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>43</v>
       </c>
@@ -8040,7 +8040,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>43</v>
       </c>
@@ -8072,7 +8072,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>43</v>
       </c>
@@ -8104,7 +8104,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>43</v>
       </c>
@@ -8136,7 +8136,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>43</v>
       </c>
@@ -8168,7 +8168,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>44</v>
       </c>
@@ -8185,7 +8185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>715</v>
       </c>
@@ -8214,7 +8214,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>715</v>
       </c>
@@ -8243,7 +8243,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>807</v>
       </c>
@@ -8263,7 +8263,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>796</v>
       </c>
@@ -8295,7 +8295,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>796</v>
       </c>
@@ -8327,7 +8327,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>796</v>
       </c>
@@ -8359,7 +8359,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>796</v>
       </c>
@@ -8391,7 +8391,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>796</v>
       </c>
@@ -8423,7 +8423,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>797</v>
       </c>
@@ -8455,7 +8455,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>797</v>
       </c>
@@ -8487,7 +8487,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>797</v>
       </c>
@@ -8519,7 +8519,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>797</v>
       </c>
@@ -8551,7 +8551,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>797</v>
       </c>
@@ -8583,7 +8583,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>798</v>
       </c>
@@ -8615,7 +8615,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>798</v>
       </c>
@@ -8647,7 +8647,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>798</v>
       </c>
@@ -8679,7 +8679,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>798</v>
       </c>
@@ -8711,7 +8711,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>798</v>
       </c>
@@ -8743,7 +8743,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>799</v>
       </c>
@@ -8775,7 +8775,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>799</v>
       </c>
@@ -8807,7 +8807,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>799</v>
       </c>
@@ -8839,7 +8839,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>799</v>
       </c>
@@ -8871,7 +8871,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>799</v>
       </c>
@@ -8903,7 +8903,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>799</v>
       </c>
@@ -8935,7 +8935,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>800</v>
       </c>
@@ -8945,11 +8945,17 @@
       <c r="C199">
         <v>1215</v>
       </c>
+      <c r="D199">
+        <v>0</v>
+      </c>
+      <c r="E199">
+        <v>0</v>
+      </c>
       <c r="I199" t="s">
         <v>710</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>801</v>
       </c>
@@ -8969,7 +8975,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>802</v>
       </c>
@@ -8989,7 +8995,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>803</v>
       </c>
@@ -9012,7 +9018,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>805</v>
       </c>
@@ -9029,7 +9035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>806</v>
       </c>

</xml_diff>